<commit_message>
Single Sign-On (SSO) with Facebook
</commit_message>
<xml_diff>
--- a/CreateSalesforceDevOrg.xlsx
+++ b/CreateSalesforceDevOrg.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vudinhquang/Documents/quang/salesforce-experience/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A5854FB-6C8C-2F4B-8052-3C94155CC0A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{130BDF61-7522-6E40-8AE9-A05D21420F4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1340" yWindow="1480" windowWidth="30600" windowHeight="18160" xr2:uid="{BCE3440F-F86F-E04D-B287-F8444623893D}"/>
+    <workbookView xWindow="39980" yWindow="2480" windowWidth="30600" windowHeight="18160" xr2:uid="{BCE3440F-F86F-E04D-B287-F8444623893D}"/>
   </bookViews>
   <sheets>
     <sheet name="Account" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="11">
   <si>
     <t>Email</t>
   </si>
@@ -56,6 +56,18 @@
   </si>
   <si>
     <t>url</t>
+  </si>
+  <si>
+    <t>hust-dev-ed.develop.my.site.com/s</t>
+  </si>
+  <si>
+    <t>12345678q</t>
+  </si>
+  <si>
+    <t>vudinhquangk53@gmail.com</t>
+  </si>
+  <si>
+    <t>Community</t>
   </si>
 </sst>
 </file>
@@ -79,7 +91,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -87,13 +99,105 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -607,47 +711,88 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8845CA88-B801-9C49-BE59-4508E8CAA659}">
-  <dimension ref="B4:C8"/>
+  <dimension ref="B3:M8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="I3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>0</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="I4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="K4" s="4"/>
+      <c r="L4" s="4"/>
+      <c r="M4" s="5"/>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>1</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="I5" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="J5" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="K5" s="8"/>
+      <c r="L5" s="8"/>
+      <c r="M5" s="9"/>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>2</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="I6" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="J6" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="K6" s="8"/>
+      <c r="L6" s="8"/>
+      <c r="M6" s="9"/>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>6</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="I7" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="J7" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="K7" s="12"/>
+      <c r="L7" s="12"/>
+      <c r="M7" s="13"/>
     </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:13" x14ac:dyDescent="0.2">
       <c r="C8" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Page Variations and Flows
</commit_message>
<xml_diff>
--- a/CreateSalesforceDevOrg.xlsx
+++ b/CreateSalesforceDevOrg.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vudinhquang/Documents/quang/salesforce-experience/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{130BDF61-7522-6E40-8AE9-A05D21420F4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1AC5269-2104-B049-B988-1A7E332841DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="39980" yWindow="2480" windowWidth="30600" windowHeight="18160" xr2:uid="{BCE3440F-F86F-E04D-B287-F8444623893D}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="13">
   <si>
     <t>Email</t>
   </si>
@@ -68,6 +68,12 @@
   </si>
   <si>
     <t>Community</t>
+  </si>
+  <si>
+    <t>vudinhquangk53+experiencecloud@gmail.com</t>
+  </si>
+  <si>
+    <t>→</t>
   </si>
 </sst>
 </file>
@@ -191,13 +197,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -221,13 +227,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>176695</xdr:colOff>
-      <xdr:row>8</xdr:row>
+      <xdr:row>10</xdr:row>
       <xdr:rowOff>110434</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
       <xdr:colOff>320260</xdr:colOff>
-      <xdr:row>75</xdr:row>
+      <xdr:row>77</xdr:row>
       <xdr:rowOff>94979</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -271,13 +277,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>165651</xdr:colOff>
-      <xdr:row>76</xdr:row>
+      <xdr:row>78</xdr:row>
       <xdr:rowOff>110435</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
       <xdr:colOff>265042</xdr:colOff>
-      <xdr:row>111</xdr:row>
+      <xdr:row>113</xdr:row>
       <xdr:rowOff>29949</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -315,14 +321,14 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>154609</xdr:colOff>
-      <xdr:row>112</xdr:row>
+      <xdr:row>114</xdr:row>
       <xdr:rowOff>121479</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
       <xdr:colOff>408608</xdr:colOff>
-      <xdr:row>170</xdr:row>
-      <xdr:rowOff>89411</xdr:rowOff>
+      <xdr:row>172</xdr:row>
+      <xdr:rowOff>89410</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -365,13 +371,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>198782</xdr:colOff>
-      <xdr:row>171</xdr:row>
+      <xdr:row>173</xdr:row>
       <xdr:rowOff>99391</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>88348</xdr:colOff>
-      <xdr:row>220</xdr:row>
+      <xdr:row>222</xdr:row>
       <xdr:rowOff>46854</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -711,10 +717,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8845CA88-B801-9C49-BE59-4508E8CAA659}">
-  <dimension ref="B3:M8"/>
+  <dimension ref="B3:M10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -743,57 +749,77 @@
     </row>
     <row r="5" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="I5" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="J5" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="K5" s="8"/>
-      <c r="L5" s="8"/>
-      <c r="M5" s="9"/>
+        <v>11</v>
+      </c>
+      <c r="I5" s="6"/>
+      <c r="J5" s="12"/>
+      <c r="K5" s="13"/>
+      <c r="L5" s="13"/>
+      <c r="M5" s="7"/>
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="J6" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="K6" s="8"/>
-      <c r="L6" s="8"/>
-      <c r="M6" s="9"/>
+        <v>1</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="M6" s="7"/>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="I7" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="J7" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="K7" s="12"/>
-      <c r="L7" s="12"/>
-      <c r="M7" s="13"/>
+        <v>11</v>
+      </c>
+      <c r="I7" s="6"/>
+      <c r="J7" s="1"/>
+      <c r="M7" s="7"/>
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="C8" s="1"/>
+      <c r="B8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I8" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="J8" t="s">
+        <v>8</v>
+      </c>
+      <c r="M8" s="7"/>
+    </row>
+    <row r="9" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I9" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="J9" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="K9" s="10"/>
+      <c r="L9" s="10"/>
+      <c r="M9" s="11"/>
+    </row>
+    <row r="10" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="C10" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Installing the Reports and Dashboards Package
</commit_message>
<xml_diff>
--- a/CreateSalesforceDevOrg.xlsx
+++ b/CreateSalesforceDevOrg.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vudinhquang/Documents/quang/salesforce-experience/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1AC5269-2104-B049-B988-1A7E332841DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{309B07AB-53FB-3449-9261-03D1CD08EA2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="39980" yWindow="2480" windowWidth="30600" windowHeight="18160" xr2:uid="{BCE3440F-F86F-E04D-B287-F8444623893D}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="14">
   <si>
     <t>Email</t>
   </si>
@@ -74,14 +74,25 @@
   </si>
   <si>
     <t>→</t>
+  </si>
+  <si>
+    <t>Salesforce Stack Exchange</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -189,7 +200,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -202,8 +213,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -717,20 +730,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8845CA88-B801-9C49-BE59-4508E8CAA659}">
-  <dimension ref="B3:M10"/>
+  <dimension ref="B3:S10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="H4" sqref="H3:H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="3" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:19" x14ac:dyDescent="0.2">
       <c r="I3" t="s">
         <v>10</v>
       </c>
+      <c r="O3" t="s">
+        <v>13</v>
+      </c>
+      <c r="P3" s="1"/>
     </row>
-    <row r="4" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>0</v>
       </c>
@@ -746,8 +763,15 @@
       <c r="K4" s="4"/>
       <c r="L4" s="4"/>
       <c r="M4" s="5"/>
+      <c r="O4" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="P4" s="3"/>
+      <c r="Q4" s="4"/>
+      <c r="R4" s="4"/>
+      <c r="S4" s="5"/>
     </row>
-    <row r="5" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>12</v>
       </c>
@@ -755,12 +779,17 @@
         <v>11</v>
       </c>
       <c r="I5" s="6"/>
-      <c r="J5" s="12"/>
-      <c r="K5" s="13"/>
-      <c r="L5" s="13"/>
+      <c r="J5" s="1"/>
       <c r="M5" s="7"/>
+      <c r="O5" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="P5" s="13"/>
+      <c r="Q5" s="12"/>
+      <c r="R5" s="12"/>
+      <c r="S5" s="7"/>
     </row>
-    <row r="6" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>1</v>
       </c>
@@ -774,8 +803,13 @@
         <v>9</v>
       </c>
       <c r="M6" s="7"/>
+      <c r="O6" s="8"/>
+      <c r="P6" s="9"/>
+      <c r="Q6" s="10"/>
+      <c r="R6" s="10"/>
+      <c r="S6" s="11"/>
     </row>
-    <row r="7" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>12</v>
       </c>
@@ -786,7 +820,7 @@
       <c r="J7" s="1"/>
       <c r="M7" s="7"/>
     </row>
-    <row r="8" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>2</v>
       </c>
@@ -801,7 +835,7 @@
       </c>
       <c r="M8" s="7"/>
     </row>
-    <row r="9" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>6</v>
       </c>
@@ -818,7 +852,7 @@
       <c r="L9" s="10"/>
       <c r="M9" s="11"/>
     </row>
-    <row r="10" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:19" x14ac:dyDescent="0.2">
       <c r="C10" s="1"/>
     </row>
   </sheetData>

</xml_diff>